<commit_message>
V2.0 Instrumento Medicion de Metricas
</commit_message>
<xml_diff>
--- a/auditoria/Instrumento_Medicion_Metricas.xlsx
+++ b/auditoria/Instrumento_Medicion_Metricas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="Ponderaciones" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Graficas (En Construccion)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="145">
   <si>
     <t>CARACTERISTICAS</t>
   </si>
@@ -360,159 +359,171 @@
 B = Casos de uso que no funcionan de la forma esperada</t>
   </si>
   <si>
-    <t>X=B-A
+    <t>Tiempo promedio en procesamiento de transaccion</t>
+  </si>
+  <si>
+    <t>Consumo promedio de memoria ram.</t>
+  </si>
+  <si>
+    <t>Cantidad de usuarios que puede atender concurrentemente</t>
+  </si>
+  <si>
+    <t>Numero de modulos con los que hay comunicacion</t>
+  </si>
+  <si>
+    <t>No Aplica</t>
+  </si>
+  <si>
+    <t>Funciones evidentes</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>Grado de satisfaccion con la navegacion del sitio</t>
+  </si>
+  <si>
+    <t>Cantidad de errores cometidos</t>
+  </si>
+  <si>
+    <t>Grado de satisfaccion del usuario con la interfaz grafica</t>
+  </si>
+  <si>
+    <t>Cantidad de operaciones empezadas y finalizadas a la semana</t>
+  </si>
+  <si>
+    <t>Cantidad de casos de uso ligados entre si</t>
+  </si>
+  <si>
+    <t>Tiempo medio de recuperacion</t>
+  </si>
+  <si>
+    <t>Porcentaje de disponibilidad diario</t>
+  </si>
+  <si>
+    <t>Numero de funciones visibles por usuario</t>
+  </si>
+  <si>
+    <t>Porcentaje de pruebas de autorización por roles</t>
+  </si>
+  <si>
+    <t>Control de accesos</t>
+  </si>
+  <si>
+    <t>Razón de ataques detectados y denegados</t>
+  </si>
+  <si>
+    <t>X = Ad/At 
+Ad = Ataques detenidos por la aplicacion 
+At = Ataques totales detectados por la aplicación</t>
+  </si>
+  <si>
+    <t>X = Pr/Pt 
+Pr = Pruebas de autorizacion realizadas
+Pt = Pruebas de autorizacion totales identificadas</t>
+  </si>
+  <si>
+    <t>Porcentaje de modulos intercambiables</t>
+  </si>
+  <si>
+    <t>Porcentaje de modulos reusables</t>
+  </si>
+  <si>
+    <t>Registro de cambios</t>
+  </si>
+  <si>
+    <t>Porcentaje de bugs detectados y corregidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X = Mr/Mt 
+Mr = Cantidad de Modulos que pueden ser reemplazables
+Mt = Cantidad de Modulos totales de la aplicacion </t>
+  </si>
+  <si>
+    <t>X = A/B
+A = Cantidad de módulos reusables en otros proyectos.
+B = Cantidad de módulos que componen el software.</t>
+  </si>
+  <si>
+    <t>X = A/B
+A = Numero de cambios a funciones o módulos que tienen comentarios
+B = Total de funciones o módulos modificados</t>
+  </si>
+  <si>
+    <t>X = A/B 
+A = Cantidad de bugs corregidos
+B = Cantidad de bugs que se han encontrado de acuerdo a las pruebas realizadas.</t>
+  </si>
+  <si>
+    <t>Tipos de dispositivos en los que se puede visualizar</t>
+  </si>
+  <si>
+    <t>X = A/B
+A = Cantidad de resoluciones en las que podrá ser visualizada la aplicación con responsive.
+B = Cantidad de resoluciones convencionales para pc y dispositivos móviles.</t>
+  </si>
+  <si>
+    <t>X=(B-A)/B
 A = Tiempo empleado en la forma actual
 B = Tiempo empleado a través de la plataforma</t>
   </si>
   <si>
-    <t>Tiempo promedio en procesamiento de transaccion</t>
-  </si>
-  <si>
-    <t>Consumo promedio de memoria ram.</t>
-  </si>
-  <si>
-    <t>Cantidad de usuarios que puede atender concurrentemente</t>
-  </si>
-  <si>
-    <t>X= Tf - T0
+    <t>X= (Tf - T0)/Tf
 T0 = Tiempo inicial en el que empieza la operacion
 Tf = Tiempo final en el cual la transaccion ha terminado</t>
   </si>
   <si>
-    <t>X = Consumo (MB)</t>
-  </si>
-  <si>
-    <t>X = Tope de usuarios</t>
-  </si>
-  <si>
-    <t>Numero de modulos con los que hay comunicacion</t>
-  </si>
-  <si>
-    <t>No Aplica</t>
-  </si>
-  <si>
-    <t>X = Cantidad de modulos</t>
-  </si>
-  <si>
-    <t>Funciones evidentes</t>
-  </si>
-  <si>
-    <t>No aplica</t>
-  </si>
-  <si>
-    <t>Grado de satisfaccion con la navegacion del sitio</t>
-  </si>
-  <si>
-    <t>Cantidad de errores cometidos</t>
-  </si>
-  <si>
-    <t>Grado de satisfaccion del usuario con la interfaz grafica</t>
-  </si>
-  <si>
-    <t>X = Cantidad de funciones evidentes</t>
-  </si>
-  <si>
-    <t>X=1=Insatisfecho, X=2=Poco Satisfecho, X=3=  Medianamente Satisfecho, X=4=Satisfecho, X=5=Muy Satisfecho</t>
-  </si>
-  <si>
-    <t>X = Cantidad de errores cometidos por usuario</t>
-  </si>
-  <si>
-    <t>Cantidad de operaciones empezadas y finalizadas a la semana</t>
-  </si>
-  <si>
-    <t>Cantidad de casos de uso ligados entre si</t>
-  </si>
-  <si>
-    <t>Tiempo medio de recuperacion</t>
-  </si>
-  <si>
-    <t>X = Cantidad de operaciones</t>
-  </si>
-  <si>
-    <t>Porcentaje de disponibilidad diario</t>
-  </si>
-  <si>
-    <t>X = A/(Tc+Tr )
+    <t>X = Consumo (MB) / Capacidad</t>
+  </si>
+  <si>
+    <t>X = Tope de usuarios/Cantidad esperada</t>
+  </si>
+  <si>
+    <t>X = Cantidad de modulos/Cantidad total de modulos</t>
+  </si>
+  <si>
+    <t>X = Cantidad de funciones evidentes/Funcionalidades Totales</t>
+  </si>
+  <si>
+    <t>X=1=Insatisfecho, X=2=Poco Satisfecho, X=3=  Medianamente Satisfecho, X=4=Satisfecho, X=5=Muy Satisfecho; X=X/5</t>
+  </si>
+  <si>
+    <t>X = Cantidad de errores con software/ Cantidad de errores sin software</t>
+  </si>
+  <si>
+    <t>X = Cantidad de operaciones terminadas/Cantidad de operaciones empezadas</t>
+  </si>
+  <si>
+    <t>X=(B-A)/B
+A = Tiempo en que el sistema tuvo una pérdida de datos o interrupción
+B = Tiempo en el que el servicio fue reestablecido</t>
+  </si>
+  <si>
+    <t>X = 1 - [ (Tc+Tr )/A ]
 A = Cantidad de horas en las que se toma la medición (24 horas)
 Tc = Tiempo que dura la falla
 Tr = Tiempo que dura la reparacion de la falla</t>
   </si>
   <si>
-    <t>X = Cantidad de casos de uso ligados</t>
-  </si>
-  <si>
-    <t>X=B-A
-A = Tiempo en que el sistema tuvo una pérdida de datos o interrupción
-B = Tiempo en el que el servicio fue reestablecido</t>
-  </si>
-  <si>
-    <t>Numero de funciones visibles por usuario</t>
-  </si>
-  <si>
-    <t>Porcentaje de pruebas de autorización por roles</t>
-  </si>
-  <si>
-    <t>Control de accesos</t>
-  </si>
-  <si>
-    <t>X = Cantidad de funciones adicionales</t>
-  </si>
-  <si>
-    <t>Razón de ataques detectados y denegados</t>
-  </si>
-  <si>
-    <t>X = Ad/At 
-Ad = Ataques detenidos por la aplicacion 
-At = Ataques totales detectados por la aplicación</t>
-  </si>
-  <si>
-    <t>X = Pr/Pt 
-Pr = Pruebas de autorizacion realizadas
-Pt = Pruebas de autorizacion totales identificadas</t>
-  </si>
-  <si>
-    <t>X = Numero de accesos a la funcionalidad</t>
-  </si>
-  <si>
-    <t>Porcentaje de modulos intercambiables</t>
-  </si>
-  <si>
-    <t>Porcentaje de modulos reusables</t>
-  </si>
-  <si>
-    <t>Registro de cambios</t>
-  </si>
-  <si>
-    <t>Porcentaje de bugs detectados y corregidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X = Mr/Mt 
-Mr = Cantidad de Modulos que pueden ser reemplazables
-Mt = Cantidad de Modulos totales de la aplicacion </t>
-  </si>
-  <si>
-    <t>X = A/B
-A = Cantidad de módulos reusables en otros proyectos.
-B = Cantidad de módulos que componen el software.</t>
-  </si>
-  <si>
-    <t>X = A/B
-A = Numero de cambios a funciones o módulos que tienen comentarios
-B = Total de funciones o módulos modificados</t>
-  </si>
-  <si>
-    <t>X = A/B 
-A = Cantidad de bugs corregidos
-B = Cantidad de bugs que se han encontrado de acuerdo a las pruebas realizadas.</t>
-  </si>
-  <si>
-    <t>Tipos de dispositivos en los que se puede visualizar</t>
-  </si>
-  <si>
-    <t>X = A/B
-A = Cantidad de resoluciones en las que podrá ser visualizada la aplicación con responsive.
-B = Cantidad de resoluciones convencionales para pc y dispositivos móviles.</t>
+    <t>X = Cantidad de casos de uso ligados/Cantidad total de casos de uso</t>
+  </si>
+  <si>
+    <t>X = Cantidad de funciones adicionales/Cantidad de funciones disponibles</t>
+  </si>
+  <si>
+    <t>X = Numero de accesos fallidos/Numero de accesos exitosos</t>
+  </si>
+  <si>
+    <t>AUD018</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -746,7 +757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -804,43 +815,45 @@
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis2" xfId="1" builtinId="33"/>
@@ -1128,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E50"/>
+  <dimension ref="B1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,6 +1156,20 @@
     <col min="5" max="5" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
     <row r="2" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1169,7 +1196,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1183,7 +1210,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="22"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1195,7 +1222,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1207,11 +1234,11 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="13">
         <f>SUM(E4:E6)</f>
         <v>1</v>
@@ -1232,7 +1259,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1246,7 +1273,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1258,7 +1285,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
@@ -1270,11 +1297,11 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="21"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="13">
         <f>SUM(E9:E11)</f>
         <v>1</v>
@@ -1295,7 +1322,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1309,7 +1336,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
@@ -1321,11 +1348,11 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="21" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="13">
         <f>SUM(E14:E15)</f>
         <v>1</v>
@@ -1346,7 +1373,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="27" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1360,7 +1387,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="7" t="s">
         <v>30</v>
       </c>
@@ -1372,7 +1399,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="7" t="s">
         <v>31</v>
       </c>
@@ -1384,7 +1411,7 @@
       </c>
     </row>
     <row r="21" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="7" t="s">
         <v>32</v>
       </c>
@@ -1396,7 +1423,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
@@ -1408,7 +1435,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="7" t="s">
         <v>33</v>
       </c>
@@ -1420,11 +1447,11 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="22"/>
-      <c r="C24" s="21" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="21"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="13">
         <f>SUM(E18:E23)</f>
         <v>1.0000000000000002</v>
@@ -1445,7 +1472,7 @@
       </c>
     </row>
     <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1459,7 +1486,7 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="22"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="7" t="s">
         <v>47</v>
       </c>
@@ -1471,7 +1498,7 @@
       </c>
     </row>
     <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="22"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="7" t="s">
         <v>48</v>
       </c>
@@ -1483,7 +1510,7 @@
       </c>
     </row>
     <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="22"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="7" t="s">
         <v>51</v>
       </c>
@@ -1495,11 +1522,11 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
-      <c r="C30" s="21" t="s">
+      <c r="B30" s="27"/>
+      <c r="C30" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="21"/>
+      <c r="D30" s="26"/>
       <c r="E30" s="13">
         <f>SUM(E26:E29)</f>
         <v>1</v>
@@ -1520,7 +1547,7 @@
       </c>
     </row>
     <row r="32" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="27" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -1534,7 +1561,7 @@
       </c>
     </row>
     <row r="33" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="22"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="7" t="s">
         <v>56</v>
       </c>
@@ -1546,7 +1573,7 @@
       </c>
     </row>
     <row r="34" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="22"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="7" t="s">
         <v>58</v>
       </c>
@@ -1558,7 +1585,7 @@
       </c>
     </row>
     <row r="35" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="22"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="7" t="s">
         <v>69</v>
       </c>
@@ -1570,7 +1597,7 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="22"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="7" t="s">
         <v>62</v>
       </c>
@@ -1582,11 +1609,11 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="22"/>
-      <c r="C37" s="21" t="s">
+      <c r="B37" s="27"/>
+      <c r="C37" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="21"/>
+      <c r="D37" s="26"/>
       <c r="E37" s="13">
         <f>SUM(E32:E36)</f>
         <v>1</v>
@@ -1607,7 +1634,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -1621,7 +1648,7 @@
       </c>
     </row>
     <row r="40" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="22"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="7" t="s">
         <v>60</v>
       </c>
@@ -1633,7 +1660,7 @@
       </c>
     </row>
     <row r="41" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="22"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="7" t="s">
         <v>71</v>
       </c>
@@ -1645,7 +1672,7 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="22"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="7" t="s">
         <v>72</v>
       </c>
@@ -1657,7 +1684,7 @@
       </c>
     </row>
     <row r="43" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="22"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="7" t="s">
         <v>74</v>
       </c>
@@ -1669,11 +1696,11 @@
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="22"/>
-      <c r="C44" s="21" t="s">
+      <c r="B44" s="27"/>
+      <c r="C44" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="21"/>
+      <c r="D44" s="26"/>
       <c r="E44" s="13">
         <f>SUM(E39:E43)</f>
         <v>1</v>
@@ -1694,7 +1721,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="27" t="s">
         <v>79</v>
       </c>
       <c r="C46" s="7" t="s">
@@ -1708,7 +1735,7 @@
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="22"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="7" t="s">
         <v>80</v>
       </c>
@@ -1720,7 +1747,7 @@
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="22"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="7" t="s">
         <v>82</v>
       </c>
@@ -1732,11 +1759,11 @@
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="22"/>
-      <c r="C49" s="21" t="s">
+      <c r="B49" s="27"/>
+      <c r="C49" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="21"/>
+      <c r="D49" s="26"/>
       <c r="E49" s="13">
         <f>SUM(E46:E48)</f>
         <v>1</v>
@@ -1777,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K43"/>
+  <dimension ref="B2:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K39" sqref="K39:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,25 +1824,25 @@
     <col min="11" max="11" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23" t="s">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-    </row>
-    <row r="3" spans="2:11" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+    </row>
+    <row r="3" spans="2:12" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
       <c r="C3" s="17" t="s">
         <v>85</v>
@@ -1835,23 +1862,23 @@
       </c>
       <c r="I3" s="30"/>
       <c r="J3" s="31"/>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="33">
         <f>SUM(H4:H6)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="33">
         <f>+Ponderaciones!D3</f>
         <v>0.16</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="33">
         <f>+C4*D4</f>
         <v>0</v>
       </c>
@@ -1866,19 +1893,20 @@
         <f>+G4*K4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="22" t="s">
         <v>91</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>95</v>
       </c>
       <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="2:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="27"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1890,7 +1918,7 @@
         <f>+G5*K5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="22" t="s">
         <v>92</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -1898,11 +1926,11 @@
       </c>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="2:11" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+    <row r="6" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="27"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1911,42 +1939,42 @@
         <v>0.2</v>
       </c>
       <c r="H6" s="13">
-        <f>+G6*K6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="26" t="s">
+        <f>(G6*K6)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="23" t="s">
         <v>93</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="2:11" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-    </row>
-    <row r="8" spans="2:11" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+    </row>
+    <row r="8" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="33">
         <f>SUM(H8:H10)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="33">
         <f>+Ponderaciones!D8</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="33">
         <f>+C8*D8</f>
         <v>0</v>
       </c>
@@ -1961,19 +1989,19 @@
         <f>+G8*K8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="25" t="s">
-        <v>98</v>
+      <c r="I8" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="2:11" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="22"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+    <row r="9" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="27"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1985,19 +2013,19 @@
         <f>+G9*K9</f>
         <v>0</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>99</v>
+      <c r="I9" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="2:11" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="22"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
+    <row r="10" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="27"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="7" t="s">
         <v>18</v>
       </c>
@@ -2009,31 +2037,39 @@
         <f>+G10*K10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="26" t="s">
-        <v>100</v>
+      <c r="I10" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29"/>
-      <c r="E11" s="29"/>
-    </row>
-    <row r="12" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="28"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+    </row>
+    <row r="12" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="33">
         <f>SUM(H12:H13)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="33">
         <f>+Ponderaciones!D13</f>
         <v>0.1</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="33">
         <f>+C12*D12</f>
         <v>0</v>
       </c>
@@ -2048,19 +2084,17 @@
         <f>+G12*K12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="32" t="s">
-        <v>105</v>
+      <c r="I12" s="24" t="s">
+        <v>101</v>
       </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
       <c r="F13" s="7" t="s">
         <v>24</v>
       </c>
@@ -2072,31 +2106,39 @@
         <f>+G13*K13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="32" t="s">
-        <v>104</v>
+      <c r="I13" s="24" t="s">
+        <v>100</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="29"/>
-      <c r="E14" s="29"/>
-    </row>
-    <row r="15" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="28"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+    </row>
+    <row r="15" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="33">
         <f>SUM(H15:H20)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="33">
         <f>+Ponderaciones!D17</f>
         <v>0.15</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="33">
         <f>+D15*C15</f>
         <v>0</v>
       </c>
@@ -2111,19 +2153,19 @@
         <f>+G15*K15</f>
         <v>0</v>
       </c>
-      <c r="I15" s="32" t="s">
-        <v>107</v>
+      <c r="I15" s="24" t="s">
+        <v>102</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
+    <row r="16" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="27"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="7" t="s">
         <v>30</v>
       </c>
@@ -2135,19 +2177,17 @@
         <f t="shared" ref="H16:H20" si="0">+G16*K16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="32" t="s">
-        <v>108</v>
+      <c r="I16" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="J16" s="3"/>
-      <c r="K16" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="2:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="27"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="7" t="s">
         <v>31</v>
       </c>
@@ -2159,19 +2199,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="32" t="s">
-        <v>109</v>
+      <c r="I17" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
       <c r="F18" s="7" t="s">
         <v>32</v>
       </c>
@@ -2183,19 +2223,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="32" t="s">
-        <v>110</v>
+      <c r="I18" s="24" t="s">
+        <v>105</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
+    <row r="19" spans="2:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="27"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="7" t="s">
         <v>34</v>
       </c>
@@ -2207,19 +2247,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="32" t="s">
-        <v>111</v>
+      <c r="I19" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
       <c r="F20" s="7" t="s">
         <v>33</v>
       </c>
@@ -2231,39 +2271,37 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="32" t="s">
-        <v>105</v>
+      <c r="I20" s="24" t="s">
+        <v>101</v>
       </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="12">
-        <v>0</v>
-      </c>
+      <c r="K20" s="12"/>
     </row>
     <row r="21" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
     </row>
     <row r="22" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="33">
         <f>SUM(H22:H25)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D22" s="33">
         <f>+Ponderaciones!D25</f>
         <v>0.12</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E22" s="33">
         <f>+D22*C22</f>
         <v>0</v>
       </c>
@@ -2274,23 +2312,23 @@
         <f>+Ponderaciones!E26</f>
         <v>0.3</v>
       </c>
-      <c r="H22" s="33">
+      <c r="H22" s="25">
         <f>+G22*K22</f>
         <v>0</v>
       </c>
-      <c r="I22" s="32" t="s">
-        <v>115</v>
+      <c r="I22" s="24" t="s">
+        <v>107</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="2:11" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
+    <row r="23" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="27"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="7" t="s">
         <v>47</v>
       </c>
@@ -2298,23 +2336,23 @@
         <f>+Ponderaciones!E27</f>
         <v>0.4</v>
       </c>
-      <c r="H23" s="33">
+      <c r="H23" s="25">
         <f t="shared" ref="H23:H24" si="1">+G23*K23</f>
         <v>0</v>
       </c>
-      <c r="I23" s="32" t="s">
-        <v>119</v>
+      <c r="I23" s="24" t="s">
+        <v>110</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="22"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
       <c r="F24" s="7" t="s">
         <v>48</v>
       </c>
@@ -2322,23 +2360,23 @@
         <f>+Ponderaciones!E28</f>
         <v>0.15</v>
       </c>
-      <c r="H24" s="33">
+      <c r="H24" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I24" s="32" t="s">
-        <v>116</v>
+      <c r="I24" s="24" t="s">
+        <v>108</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="22"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
       <c r="F25" s="7" t="s">
         <v>51</v>
       </c>
@@ -2346,43 +2384,43 @@
         <f>+Ponderaciones!E29</f>
         <v>0.15</v>
       </c>
-      <c r="H25" s="33">
+      <c r="H25" s="25">
         <f>+G25*K25</f>
         <v>0</v>
       </c>
-      <c r="I25" s="32" t="s">
-        <v>117</v>
+      <c r="I25" s="24" t="s">
+        <v>109</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
     </row>
     <row r="27" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="33">
         <f>SUM(H27:H31)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="33">
         <f>+Ponderaciones!D31</f>
         <v>0.15</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="33">
         <f>+D27*C27</f>
         <v>0</v>
       </c>
@@ -2393,23 +2431,23 @@
         <f>+Ponderaciones!E32</f>
         <v>0.25</v>
       </c>
-      <c r="H27" s="33">
+      <c r="H27" s="25">
         <f>+G27*K27</f>
         <v>0</v>
       </c>
-      <c r="I27" s="32" t="s">
-        <v>123</v>
+      <c r="I27" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="K27" s="12"/>
     </row>
     <row r="28" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="22"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
       <c r="F28" s="7" t="s">
         <v>56</v>
       </c>
@@ -2417,23 +2455,23 @@
         <f>+Ponderaciones!E33</f>
         <v>0.2</v>
       </c>
-      <c r="H28" s="33">
+      <c r="H28" s="25">
         <f t="shared" ref="H28:H31" si="2">+G28*K28</f>
         <v>0</v>
       </c>
-      <c r="I28" s="32" t="s">
-        <v>127</v>
+      <c r="I28" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="22"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
       <c r="F29" s="7" t="s">
         <v>58</v>
       </c>
@@ -2441,23 +2479,21 @@
         <f>+Ponderaciones!E34</f>
         <v>0.1</v>
       </c>
-      <c r="H29" s="33">
+      <c r="H29" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I29" s="32" t="s">
-        <v>108</v>
+      <c r="I29" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="J29" s="3"/>
-      <c r="K29" s="12">
-        <v>0</v>
-      </c>
+      <c r="K29" s="12"/>
     </row>
     <row r="30" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
       <c r="F30" s="7" t="s">
         <v>69</v>
       </c>
@@ -2465,23 +2501,23 @@
         <f>+Ponderaciones!E35</f>
         <v>0.2</v>
       </c>
-      <c r="H30" s="33">
+      <c r="H30" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I30" s="32" t="s">
-        <v>124</v>
+      <c r="I30" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="K30" s="12"/>
     </row>
     <row r="31" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="22"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
       <c r="F31" s="7" t="s">
         <v>62</v>
       </c>
@@ -2489,43 +2525,43 @@
         <f>+Ponderaciones!E36</f>
         <v>0.25</v>
       </c>
-      <c r="H31" s="33">
+      <c r="H31" s="25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I31" s="32" t="s">
-        <v>125</v>
+      <c r="I31" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="K31" s="12"/>
     </row>
     <row r="32" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
     </row>
     <row r="33" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="28">
+      <c r="C33" s="33">
         <f>SUM(H33:H37)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="33">
         <f>+Ponderaciones!D38</f>
         <v>0.1</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="33">
         <f>+D33*C33</f>
         <v>0</v>
       </c>
@@ -2536,23 +2572,23 @@
         <f>+Ponderaciones!E39</f>
         <v>0.3</v>
       </c>
-      <c r="H33" s="33">
+      <c r="H33" s="25">
         <f>+G33*K33</f>
         <v>0</v>
       </c>
-      <c r="I33" s="32" t="s">
-        <v>131</v>
+      <c r="I33" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="K33" s="12"/>
     </row>
     <row r="34" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="22"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
       <c r="F34" s="7" t="s">
         <v>60</v>
       </c>
@@ -2560,23 +2596,23 @@
         <f>+Ponderaciones!E40</f>
         <v>0.2</v>
       </c>
-      <c r="H34" s="33">
+      <c r="H34" s="25">
         <f t="shared" ref="H34:H37" si="3">+G34*K34</f>
         <v>0</v>
       </c>
-      <c r="I34" s="32" t="s">
-        <v>132</v>
+      <c r="I34" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="K34" s="12"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="22"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
       <c r="F35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2584,23 +2620,21 @@
         <f>+Ponderaciones!E41</f>
         <v>0.1</v>
       </c>
-      <c r="H35" s="33">
+      <c r="H35" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I35" s="32" t="s">
-        <v>108</v>
+      <c r="I35" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="J35" s="3"/>
-      <c r="K35" s="12">
-        <v>0</v>
-      </c>
+      <c r="K35" s="12"/>
     </row>
     <row r="36" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B36" s="22"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
       <c r="F36" s="7" t="s">
         <v>72</v>
       </c>
@@ -2608,23 +2642,23 @@
         <f>+Ponderaciones!E42</f>
         <v>0.2</v>
       </c>
-      <c r="H36" s="33">
+      <c r="H36" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I36" s="32" t="s">
-        <v>133</v>
+      <c r="I36" s="24" t="s">
+        <v>119</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B37" s="22"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="7" t="s">
         <v>74</v>
       </c>
@@ -2632,43 +2666,43 @@
         <f>+Ponderaciones!E43</f>
         <v>0.2</v>
       </c>
-      <c r="H37" s="33">
+      <c r="H37" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I37" s="32" t="s">
-        <v>134</v>
+      <c r="I37" s="24" t="s">
+        <v>120</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="K37" s="12"/>
     </row>
     <row r="38" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
     </row>
     <row r="39" spans="2:11" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C39" s="33">
         <f>SUM(H39:H41)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="28">
+      <c r="D39" s="33">
         <f>+Ponderaciones!D45</f>
         <v>0.08</v>
       </c>
-      <c r="E39" s="28">
+      <c r="E39" s="33">
         <f>+D39*C39</f>
         <v>0</v>
       </c>
@@ -2679,23 +2713,23 @@
         <f>+Ponderaciones!E46</f>
         <v>0.5</v>
       </c>
-      <c r="H39" s="33">
+      <c r="H39" s="25">
         <f>+G39*K39</f>
         <v>0</v>
       </c>
-      <c r="I39" s="32" t="s">
-        <v>139</v>
+      <c r="I39" s="24" t="s">
+        <v>125</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="K39" s="12"/>
     </row>
     <row r="40" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="22"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
       <c r="F40" s="7" t="s">
         <v>80</v>
       </c>
@@ -2703,23 +2737,21 @@
         <f>+Ponderaciones!E47</f>
         <v>0.2</v>
       </c>
-      <c r="H40" s="33">
+      <c r="H40" s="25">
         <f t="shared" ref="H40:H41" si="4">+G40*K40</f>
         <v>0</v>
       </c>
-      <c r="I40" s="32" t="s">
-        <v>108</v>
+      <c r="I40" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="J40" s="3"/>
-      <c r="K40" s="12">
-        <v>0</v>
-      </c>
+      <c r="K40" s="12"/>
     </row>
     <row r="41" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="22"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
       <c r="F41" s="7" t="s">
         <v>82</v>
       </c>
@@ -2727,29 +2759,27 @@
         <f>+Ponderaciones!E48</f>
         <v>0.3</v>
       </c>
-      <c r="H41" s="33">
+      <c r="H41" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I41" s="32" t="s">
-        <v>108</v>
+      <c r="I41" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="J41" s="3"/>
-      <c r="K41" s="12">
-        <v>0</v>
-      </c>
+      <c r="K41" s="12"/>
     </row>
     <row r="42" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D43" s="9">
@@ -2777,8 +2807,6 @@
     <mergeCell ref="D27:D31"/>
     <mergeCell ref="E27:E31"/>
     <mergeCell ref="B28:B31"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="E15:E20"/>
     <mergeCell ref="B26:K26"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="D22:D25"/>
@@ -2791,6 +2819,8 @@
     <mergeCell ref="B21:K21"/>
     <mergeCell ref="B16:B20"/>
     <mergeCell ref="C15:C20"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="E15:E20"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="I3:J3"/>

</xml_diff>

<commit_message>
V3.0 Instrumento de Medicion de Metricas. Agregada grafica de barras para comparar caracteristicas de calidad
</commit_message>
<xml_diff>
--- a/auditoria/Instrumento_Medicion_Metricas.xlsx
+++ b/auditoria/Instrumento_Medicion_Metricas.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Ponderaciones" sheetId="1" r:id="rId1"/>
     <sheet name="Calificacion Detalladas" sheetId="3" r:id="rId2"/>
-    <sheet name="Graficas (En Construccion)" sheetId="4" r:id="rId3"/>
+    <sheet name="Graficas" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="148">
   <si>
     <t>CARACTERISTICAS</t>
   </si>
@@ -523,14 +523,23 @@
     <t>VERSION</t>
   </si>
   <si>
-    <t>2.0</t>
+    <t>Calificacion Total</t>
+  </si>
+  <si>
+    <t>Ponderacion Total</t>
+  </si>
+  <si>
+    <t>Calificacion Ponderada Total</t>
+  </si>
+  <si>
+    <t>3.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,6 +619,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -666,7 +683,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -752,12 +769,186 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -828,15 +1019,56 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -846,14 +1078,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis2" xfId="1" builtinId="33"/>
@@ -863,8 +1090,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF29C7FF"/>
       <color rgb="FF00FFFF"/>
-      <color rgb="FF29C7FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -876,6 +1103,1118 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO" b="1"/>
+              <a:t>Comparación Características </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.31435848918205994"/>
+          <c:y val="4.3073890993764304E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graficas!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calificacion Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graficas!$B$3:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Funcionalidad</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Rendimiento</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Compatibilidad</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Usabilidad</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fiabilidad</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Seguridad</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mantenibilidad</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Portabilidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graficas!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graficas!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calificacion Ponderada Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graficas!$B$3:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Funcionalidad</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Rendimiento</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Compatibilidad</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Usabilidad</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fiabilidad</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Seguridad</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mantenibilidad</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Portabilidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graficas!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="102999240"/>
+        <c:axId val="103003160"/>
+        <c:axId val="197516688"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="102999240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103003160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="103003160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="102999240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="197516688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103003160"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19039304461942258"/>
+          <c:y val="0.78298556430446198"/>
+          <c:w val="0.61921391076115484"/>
+          <c:h val="0.18923665791776026"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>4760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>556141</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1144,7 +2483,7 @@
   <dimension ref="B1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,17 +2496,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="26" t="s">
         <v>142</v>
       </c>
       <c r="C1" t="s">
         <v>141</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="26" t="s">
         <v>143</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1196,7 +2535,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1210,7 +2549,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="27"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1222,7 +2561,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1234,11 +2573,11 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="13">
         <f>SUM(E4:E6)</f>
         <v>1</v>
@@ -1259,7 +2598,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="39" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1273,7 +2612,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1285,7 +2624,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
@@ -1297,11 +2636,11 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="13">
         <f>SUM(E9:E11)</f>
         <v>1</v>
@@ -1322,7 +2661,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="39" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1336,7 +2675,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
@@ -1348,11 +2687,11 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="26" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="26"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="13">
         <f>SUM(E14:E15)</f>
         <v>1</v>
@@ -1373,7 +2712,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="39" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1387,7 +2726,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="7" t="s">
         <v>30</v>
       </c>
@@ -1399,7 +2738,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="7" t="s">
         <v>31</v>
       </c>
@@ -1411,7 +2750,7 @@
       </c>
     </row>
     <row r="21" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="27"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="7" t="s">
         <v>32</v>
       </c>
@@ -1423,7 +2762,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="27"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="7" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +2774,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="27"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="7" t="s">
         <v>33</v>
       </c>
@@ -1447,11 +2786,11 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="27"/>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="39"/>
+      <c r="C24" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="26"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="13">
         <f>SUM(E18:E23)</f>
         <v>1.0000000000000002</v>
@@ -1472,7 +2811,7 @@
       </c>
     </row>
     <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="39" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1486,7 +2825,7 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="7" t="s">
         <v>47</v>
       </c>
@@ -1498,7 +2837,7 @@
       </c>
     </row>
     <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="27"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="7" t="s">
         <v>48</v>
       </c>
@@ -1510,7 +2849,7 @@
       </c>
     </row>
     <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="27"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="7" t="s">
         <v>51</v>
       </c>
@@ -1522,11 +2861,11 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="27"/>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="40"/>
       <c r="E30" s="13">
         <f>SUM(E26:E29)</f>
         <v>1</v>
@@ -1547,7 +2886,7 @@
       </c>
     </row>
     <row r="32" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="39" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -1561,7 +2900,7 @@
       </c>
     </row>
     <row r="33" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="27"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="7" t="s">
         <v>56</v>
       </c>
@@ -1573,7 +2912,7 @@
       </c>
     </row>
     <row r="34" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="27"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="7" t="s">
         <v>58</v>
       </c>
@@ -1585,7 +2924,7 @@
       </c>
     </row>
     <row r="35" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="27"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="7" t="s">
         <v>69</v>
       </c>
@@ -1597,7 +2936,7 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="27"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7" t="s">
         <v>62</v>
       </c>
@@ -1609,11 +2948,11 @@
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="27"/>
-      <c r="C37" s="26" t="s">
+      <c r="B37" s="39"/>
+      <c r="C37" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="26"/>
+      <c r="D37" s="40"/>
       <c r="E37" s="13">
         <f>SUM(E32:E36)</f>
         <v>1</v>
@@ -1634,7 +2973,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="39" t="s">
         <v>65</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -1648,7 +2987,7 @@
       </c>
     </row>
     <row r="40" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="27"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="7" t="s">
         <v>60</v>
       </c>
@@ -1660,7 +2999,7 @@
       </c>
     </row>
     <row r="41" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="27"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="7" t="s">
         <v>71</v>
       </c>
@@ -1672,7 +3011,7 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="27"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7" t="s">
         <v>72</v>
       </c>
@@ -1684,7 +3023,7 @@
       </c>
     </row>
     <row r="43" spans="2:5" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="27"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7" t="s">
         <v>74</v>
       </c>
@@ -1696,11 +3035,11 @@
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="27"/>
-      <c r="C44" s="26" t="s">
+      <c r="B44" s="39"/>
+      <c r="C44" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="26"/>
+      <c r="D44" s="40"/>
       <c r="E44" s="13">
         <f>SUM(E39:E43)</f>
         <v>1</v>
@@ -1721,7 +3060,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="39" t="s">
         <v>79</v>
       </c>
       <c r="C46" s="7" t="s">
@@ -1735,7 +3074,7 @@
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
+      <c r="B47" s="39"/>
       <c r="C47" s="7" t="s">
         <v>80</v>
       </c>
@@ -1747,7 +3086,7 @@
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="27"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="7" t="s">
         <v>82</v>
       </c>
@@ -1759,11 +3098,11 @@
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="27"/>
-      <c r="C49" s="26" t="s">
+      <c r="B49" s="39"/>
+      <c r="C49" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="26"/>
+      <c r="D49" s="40"/>
       <c r="E49" s="13">
         <f>SUM(E46:E48)</f>
         <v>1</v>
@@ -1780,6 +3119,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="B39:B44"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="B46:B49"/>
@@ -1790,12 +3135,6 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="B32:B37"/>
     <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1807,7 +3146,7 @@
   <dimension ref="B2:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K39" sqref="K39:K41"/>
+      <selection activeCell="K4" sqref="K4:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,22 +3164,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29" t="s">
+      <c r="B2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29" t="s">
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
     </row>
     <row r="3" spans="2:12" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
@@ -1860,8 +3199,8 @@
       <c r="H3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="21" t="s">
         <v>94</v>
       </c>
@@ -1870,15 +3209,15 @@
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="42">
         <f>SUM(H4:H6)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="42">
         <f>+Ponderaciones!D3</f>
         <v>0.16</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="42">
         <f>+C4*D4</f>
         <v>0</v>
       </c>
@@ -1903,10 +3242,10 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="2:12" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
@@ -1927,10 +3266,10 @@
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="27"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1951,30 +3290,30 @@
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="2:12" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
     </row>
     <row r="8" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="42">
         <f>SUM(H8:H10)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="42">
         <f>+Ponderaciones!D8</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="42">
         <f>+C8*D8</f>
         <v>0</v>
       </c>
@@ -1998,10 +3337,10 @@
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="7" t="s">
         <v>17</v>
       </c>
@@ -2022,10 +3361,10 @@
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="27"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="7" t="s">
         <v>18</v>
       </c>
@@ -2046,30 +3385,30 @@
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
     </row>
     <row r="12" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="42">
         <f>SUM(H12:H13)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="42">
         <f>+Ponderaciones!D13</f>
         <v>0.1</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="42">
         <f>+C12*D12</f>
         <v>0</v>
       </c>
@@ -2092,9 +3431,9 @@
     </row>
     <row r="13" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="7" t="s">
         <v>24</v>
       </c>
@@ -2115,30 +3454,30 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
     </row>
     <row r="15" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="42">
         <f>SUM(H15:H20)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="42">
         <f>+Ponderaciones!D17</f>
         <v>0.15</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="42">
         <f>+D15*C15</f>
         <v>0</v>
       </c>
@@ -2162,10 +3501,10 @@
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="7" t="s">
         <v>30</v>
       </c>
@@ -2184,10 +3523,10 @@
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="2:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="7" t="s">
         <v>31</v>
       </c>
@@ -2208,10 +3547,10 @@
       <c r="K17" s="12"/>
     </row>
     <row r="18" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="27"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="7" t="s">
         <v>32</v>
       </c>
@@ -2232,10 +3571,10 @@
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="2:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="7" t="s">
         <v>34</v>
       </c>
@@ -2256,10 +3595,10 @@
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="7" t="s">
         <v>33</v>
       </c>
@@ -2278,30 +3617,30 @@
       <c r="K20" s="12"/>
     </row>
     <row r="21" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
     </row>
     <row r="22" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C22" s="42">
         <f>SUM(H22:H25)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="42">
         <f>+Ponderaciones!D25</f>
         <v>0.12</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="42">
         <f>+D22*C22</f>
         <v>0</v>
       </c>
@@ -2325,10 +3664,10 @@
       <c r="K22" s="12"/>
     </row>
     <row r="23" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B23" s="27"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="7" t="s">
         <v>47</v>
       </c>
@@ -2349,10 +3688,10 @@
       <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="27"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="7" t="s">
         <v>48</v>
       </c>
@@ -2373,10 +3712,10 @@
       <c r="K24" s="12"/>
     </row>
     <row r="25" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="7" t="s">
         <v>51</v>
       </c>
@@ -2397,30 +3736,30 @@
       <c r="K25" s="12"/>
     </row>
     <row r="26" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="41"/>
     </row>
     <row r="27" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="42">
         <f>SUM(H27:H31)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="42">
         <f>+Ponderaciones!D31</f>
         <v>0.15</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="42">
         <f>+D27*C27</f>
         <v>0</v>
       </c>
@@ -2444,10 +3783,10 @@
       <c r="K27" s="12"/>
     </row>
     <row r="28" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="27"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="7" t="s">
         <v>56</v>
       </c>
@@ -2468,10 +3807,10 @@
       <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="27"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="7" t="s">
         <v>58</v>
       </c>
@@ -2490,10 +3829,10 @@
       <c r="K29" s="12"/>
     </row>
     <row r="30" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="27"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="7" t="s">
         <v>69</v>
       </c>
@@ -2514,10 +3853,10 @@
       <c r="K30" s="12"/>
     </row>
     <row r="31" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
       <c r="F31" s="7" t="s">
         <v>62</v>
       </c>
@@ -2538,30 +3877,30 @@
       <c r="K31" s="12"/>
     </row>
     <row r="32" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
     </row>
     <row r="33" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="33">
+      <c r="C33" s="42">
         <f>SUM(H33:H37)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="33">
+      <c r="D33" s="42">
         <f>+Ponderaciones!D38</f>
         <v>0.1</v>
       </c>
-      <c r="E33" s="33">
+      <c r="E33" s="42">
         <f>+D33*C33</f>
         <v>0</v>
       </c>
@@ -2585,10 +3924,10 @@
       <c r="K33" s="12"/>
     </row>
     <row r="34" spans="2:11" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="27"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
       <c r="F34" s="7" t="s">
         <v>60</v>
       </c>
@@ -2609,10 +3948,10 @@
       <c r="K34" s="12"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="27"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2631,10 +3970,10 @@
       <c r="K35" s="12"/>
     </row>
     <row r="36" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B36" s="27"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
       <c r="F36" s="7" t="s">
         <v>72</v>
       </c>
@@ -2655,10 +3994,10 @@
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B37" s="27"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
       <c r="F37" s="7" t="s">
         <v>74</v>
       </c>
@@ -2679,30 +4018,30 @@
       <c r="K37" s="12"/>
     </row>
     <row r="38" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
     </row>
     <row r="39" spans="2:11" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="33">
+      <c r="C39" s="42">
         <f>SUM(H39:H41)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="33">
+      <c r="D39" s="42">
         <f>+Ponderaciones!D45</f>
         <v>0.08</v>
       </c>
-      <c r="E39" s="33">
+      <c r="E39" s="42">
         <f>+D39*C39</f>
         <v>0</v>
       </c>
@@ -2726,10 +4065,10 @@
       <c r="K39" s="12"/>
     </row>
     <row r="40" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="27"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
       <c r="F40" s="7" t="s">
         <v>80</v>
       </c>
@@ -2748,10 +4087,10 @@
       <c r="K40" s="12"/>
     </row>
     <row r="41" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="27"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
       <c r="F41" s="7" t="s">
         <v>82</v>
       </c>
@@ -2770,16 +4109,16 @@
       <c r="K41" s="12"/>
     </row>
     <row r="42" spans="2:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="41"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D43" s="9">
@@ -2792,35 +4131,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="D33:D37"/>
-    <mergeCell ref="E33:E37"/>
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="E15:E20"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="I3:J3"/>
@@ -2835,6 +4145,35 @@
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="D4:D6"/>
     <mergeCell ref="E4:E6"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="D33:D37"/>
+    <mergeCell ref="E33:E37"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2843,14 +4182,174 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="33">
+        <f>'Calificacion Detalladas'!C4</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <f>'Calificacion Detalladas'!D4</f>
+        <v>0.16</v>
+      </c>
+      <c r="E3" s="34">
+        <f>'Calificacion Detalladas'!E4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="35">
+        <f>'Calificacion Detalladas'!C8</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="35">
+        <f>'Calificacion Detalladas'!D8</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E4" s="36">
+        <f>'Calificacion Detalladas'!E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="35">
+        <f>'Calificacion Detalladas'!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="35">
+        <f>'Calificacion Detalladas'!D12</f>
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="36">
+        <f>'Calificacion Detalladas'!E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="35">
+        <f>'Calificacion Detalladas'!C15</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="35">
+        <f>'Calificacion Detalladas'!D15</f>
+        <v>0.15</v>
+      </c>
+      <c r="E6" s="36">
+        <f>'Calificacion Detalladas'!E15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="35">
+        <f>'Calificacion Detalladas'!C22</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="35">
+        <f>'Calificacion Detalladas'!D22</f>
+        <v>0.12</v>
+      </c>
+      <c r="E7" s="36">
+        <f>'Calificacion Detalladas'!E22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="35">
+        <f>'Calificacion Detalladas'!C27</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="35">
+        <f>'Calificacion Detalladas'!D27</f>
+        <v>0.15</v>
+      </c>
+      <c r="E8" s="36">
+        <f>'Calificacion Detalladas'!E27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="35">
+        <f>'Calificacion Detalladas'!C33</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="35">
+        <f>'Calificacion Detalladas'!D33</f>
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="36">
+        <f>'Calificacion Detalladas'!E33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="37">
+        <f>'Calificacion Detalladas'!C39</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="37">
+        <f>'Calificacion Detalladas'!D39</f>
+        <v>0.08</v>
+      </c>
+      <c r="E10" s="38">
+        <f>'Calificacion Detalladas'!E39</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>